<commit_message>
Reset name of supplement table3;
</commit_message>
<xml_diff>
--- a/data/procon/threshold_100/group distribution statistic information.xlsx
+++ b/data/procon/threshold_100/group distribution statistic information.xlsx
@@ -53,7 +53,7 @@
     <t>index</t>
   </si>
   <si>
-    <t>Yes. Right.</t>
+    <t>Yes. Smaller.</t>
   </si>
   <si>
     <t>BA.1(Omicron)</t>
@@ -158,7 +158,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Yes. Left.</t>
+    <t>Yes. Bigger.</t>
   </si>
 </sst>
 </file>

</xml_diff>